<commit_message>
Converted Design Matrix to Include ISF as an IV
</commit_message>
<xml_diff>
--- a/Data for Thesis New Design Matrix.xlsx
+++ b/Data for Thesis New Design Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solbenishay/Desktop/School/2020:21/WInter/Thesis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5292337A-1CAC-4A4A-A22C-AC8A178DAE38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE99E6A1-DEBD-B34F-A6CE-D88397D44DAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1497,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AG4" sqref="AG4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>